<commit_message>
Added funcion to use list as leaf.
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_IndexedListColumn.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_IndexedListColumn.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\exceltable\xlbean\src\test\java\com\xlbean\reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8E63F5-4175-46E1-AA7E-E8FF06A8FEB3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8228" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="formatForceString" sheetId="5" r:id="rId1"/>
+    <sheet name="indexedList" sheetId="5" r:id="rId1"/>
+    <sheet name="indexedListAsLeaf" sheetId="6" r:id="rId2"/>
+    <sheet name="indexedListAsLeafTestOption" sheetId="7" r:id="rId3"/>
+    <sheet name="indexedListAsLeafTestLeft" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -111,13 +115,97 @@
   </si>
   <si>
     <t>key1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeaf#test</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeaf#list[0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeaf#list[1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeaf#list[2]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeaf#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#list[0]</t>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#list[2]</t>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#test?type=string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#list[1]?type=string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[0]#test?type=string</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[0]#list[0]</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[0]#list[1]?type=string</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[0]#list[2]</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[1]#list[1]?type=string</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[1]#list[2]</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[0]#~, listAsLeafTestLeft[1]#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[1]#test</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[1]#list[0]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,32 +562,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
     <col min="2" max="2" width="1.25" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.1640625" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" customWidth="1"/>
-    <col min="15" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1875" customWidth="1"/>
+    <col min="7" max="7" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1875" customWidth="1"/>
+    <col min="9" max="9" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1875" customWidth="1"/>
+    <col min="11" max="11" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1875" customWidth="1"/>
+    <col min="13" max="13" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1875" customWidth="1"/>
+    <col min="15" max="16" width="18.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.7">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -587,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C5">
         <v>2</v>
       </c>
@@ -622,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C6">
         <v>3</v>
       </c>
@@ -651,7 +739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C7">
         <v>4</v>
       </c>
@@ -668,7 +756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C8">
         <v>5</v>
       </c>
@@ -676,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C9">
         <v>6</v>
       </c>
@@ -687,7 +775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C10">
         <v>7</v>
       </c>
@@ -700,4 +788,275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2A8BB3-CC2C-4C88-AB6D-E5D6459EC306}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.6875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="E6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E1254E-808E-4F44-B5C6-D636FF442344}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.375" customWidth="1"/>
+    <col min="3" max="3" width="34.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.4375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.4375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
+      <c r="E6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD62F87-2618-4C47-83F1-32291F60E144}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.375" customWidth="1"/>
+    <col min="3" max="3" width="34.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.4375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.4375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1875" customWidth="1"/>
+    <col min="8" max="8" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.8125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="E6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Added converter option"
This reverts commit bfcc6389415308bf428fd9f3947a6c000f21529d.
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_IndexedListColumn.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_IndexedListColumn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F62E751-3712-4844-BE56-773EB466AA97}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8E63F5-4175-46E1-AA7E-E8FF06A8FEB3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="-108" windowWidth="29448" windowHeight="17496" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8228" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indexedList" sheetId="5" r:id="rId1"/>
@@ -160,16 +160,33 @@
     <t>listAsLeafTestOption#list[2]</t>
   </si>
   <si>
+    <t>listAsLeafTestOption#test?type=string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#list[1]?type=string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>listAsLeafTestOption#~</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>listAsLeafTestLeft[0]#test?type=string</t>
+  </si>
+  <si>
     <t>listAsLeafTestLeft[0]#list[0]</t>
   </si>
   <si>
+    <t>listAsLeafTestLeft[0]#list[1]?type=string</t>
+  </si>
+  <si>
     <t>listAsLeafTestLeft[0]#list[2]</t>
   </si>
   <si>
+    <t>listAsLeafTestLeft[1]#list[1]?type=string</t>
+  </si>
+  <si>
     <t>listAsLeafTestLeft[1]#list[2]</t>
   </si>
   <si>
@@ -183,21 +200,6 @@
   <si>
     <t>listAsLeafTestLeft[1]#list[0]</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>listAsLeafTestLeft[0]#test?readAs=text</t>
-  </si>
-  <si>
-    <t>listAsLeafTestLeft[0]#list[1]?readAs=text</t>
-  </si>
-  <si>
-    <t>listAsLeafTestLeft[1]#list[1]?readAs=text</t>
-  </si>
-  <si>
-    <t>listAsLeafTestOption#test?readAs=text</t>
-  </si>
-  <si>
-    <t>listAsLeafTestOption#list[1]?readAs=text</t>
   </si>
 </sst>
 </file>
@@ -567,25 +569,25 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="2" max="2" width="1.19921875" customWidth="1"/>
+    <col min="2" max="2" width="1.25" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.19921875" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.19921875" customWidth="1"/>
-    <col min="9" max="9" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.19921875" customWidth="1"/>
-    <col min="11" max="11" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.19921875" customWidth="1"/>
-    <col min="13" max="13" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.19921875" customWidth="1"/>
-    <col min="15" max="16" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1875" customWidth="1"/>
+    <col min="7" max="7" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1875" customWidth="1"/>
+    <col min="9" max="9" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1875" customWidth="1"/>
+    <col min="11" max="11" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1875" customWidth="1"/>
+    <col min="13" max="13" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1875" customWidth="1"/>
+    <col min="15" max="16" width="18.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.7">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -673,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C5">
         <v>2</v>
       </c>
@@ -708,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C6">
         <v>3</v>
       </c>
@@ -737,7 +739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C7">
         <v>4</v>
       </c>
@@ -754,7 +756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C8">
         <v>5</v>
       </c>
@@ -762,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C9">
         <v>6</v>
       </c>
@@ -773,7 +775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.7">
       <c r="C10">
         <v>7</v>
       </c>
@@ -792,17 +794,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2A8BB3-CC2C-4C88-AB6D-E5D6459EC306}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="3" max="3" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +821,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -836,7 +838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
       <c r="D4">
         <v>1</v>
       </c>
@@ -847,7 +849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.7">
       <c r="D5">
         <v>4</v>
       </c>
@@ -855,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
       <c r="E6">
         <v>6</v>
       </c>
@@ -874,36 +876,36 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.3984375" customWidth="1"/>
-    <col min="3" max="3" width="34.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.375" customWidth="1"/>
+    <col min="3" max="3" width="34.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.4375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.4375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -918,7 +920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
       <c r="D4">
         <v>1</v>
       </c>
@@ -929,7 +931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.7">
       <c r="D5">
         <v>4</v>
       </c>
@@ -937,7 +939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
       <c r="E6">
         <v>6</v>
       </c>
@@ -952,57 +954,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD62F87-2618-4C47-83F1-32291F60E144}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.3984375" customWidth="1"/>
-    <col min="3" max="3" width="34.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.19921875" customWidth="1"/>
-    <col min="8" max="8" width="23.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.375" customWidth="1"/>
+    <col min="3" max="3" width="34.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.4375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.4375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1875" customWidth="1"/>
+    <col min="8" max="8" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.8125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
         <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>37</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1029,7 +1031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.7">
       <c r="D4">
         <v>1</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.7">
       <c r="D5">
         <v>4</v>
       </c>
@@ -1048,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.7">
       <c r="E6">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
#53 Added converter option
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_IndexedListColumn.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_IndexedListColumn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8E63F5-4175-46E1-AA7E-E8FF06A8FEB3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F62E751-3712-4844-BE56-773EB466AA97}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8228" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="-108" windowWidth="29448" windowHeight="17496" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indexedList" sheetId="5" r:id="rId1"/>
@@ -160,33 +160,16 @@
     <t>listAsLeafTestOption#list[2]</t>
   </si>
   <si>
-    <t>listAsLeafTestOption#test?type=string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>listAsLeafTestOption#list[1]?type=string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>listAsLeafTestOption#~</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>listAsLeafTestLeft[0]#test?type=string</t>
-  </si>
-  <si>
     <t>listAsLeafTestLeft[0]#list[0]</t>
   </si>
   <si>
-    <t>listAsLeafTestLeft[0]#list[1]?type=string</t>
-  </si>
-  <si>
     <t>listAsLeafTestLeft[0]#list[2]</t>
   </si>
   <si>
-    <t>listAsLeafTestLeft[1]#list[1]?type=string</t>
-  </si>
-  <si>
     <t>listAsLeafTestLeft[1]#list[2]</t>
   </si>
   <si>
@@ -200,6 +183,21 @@
   <si>
     <t>listAsLeafTestLeft[1]#list[0]</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[0]#test?readAs=text</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[0]#list[1]?readAs=text</t>
+  </si>
+  <si>
+    <t>listAsLeafTestLeft[1]#list[1]?readAs=text</t>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#test?readAs=text</t>
+  </si>
+  <si>
+    <t>listAsLeafTestOption#list[1]?readAs=text</t>
   </si>
 </sst>
 </file>
@@ -569,25 +567,25 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="1.25" customWidth="1"/>
+    <col min="2" max="2" width="1.19921875" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.8125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1875" customWidth="1"/>
-    <col min="7" max="7" width="18.8125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1875" customWidth="1"/>
-    <col min="9" max="9" width="18.8125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1875" customWidth="1"/>
-    <col min="11" max="11" width="18.8125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.1875" customWidth="1"/>
-    <col min="13" max="13" width="18.8125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1875" customWidth="1"/>
-    <col min="15" max="16" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.19921875" customWidth="1"/>
+    <col min="9" max="9" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.19921875" customWidth="1"/>
+    <col min="11" max="11" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.19921875" customWidth="1"/>
+    <col min="13" max="13" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.19921875" customWidth="1"/>
+    <col min="15" max="16" width="18.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -675,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C5">
         <v>2</v>
       </c>
@@ -710,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C6">
         <v>3</v>
       </c>
@@ -739,7 +737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C7">
         <v>4</v>
       </c>
@@ -756,7 +754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>5</v>
       </c>
@@ -764,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C9">
         <v>6</v>
       </c>
@@ -775,7 +773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C10">
         <v>7</v>
       </c>
@@ -794,17 +792,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2A8BB3-CC2C-4C88-AB6D-E5D6459EC306}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="15.6875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -838,7 +836,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D4">
         <v>1</v>
       </c>
@@ -849,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5">
         <v>4</v>
       </c>
@@ -857,7 +855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E6">
         <v>6</v>
       </c>
@@ -876,36 +874,36 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.375" customWidth="1"/>
-    <col min="3" max="3" width="34.8125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.4375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.4375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.3984375" customWidth="1"/>
+    <col min="3" max="3" width="34.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -920,7 +918,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D4">
         <v>1</v>
       </c>
@@ -931,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5">
         <v>4</v>
       </c>
@@ -939,7 +937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E6">
         <v>6</v>
       </c>
@@ -954,57 +952,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD62F87-2618-4C47-83F1-32291F60E144}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.375" customWidth="1"/>
-    <col min="3" max="3" width="34.8125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.4375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.4375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1875" customWidth="1"/>
-    <col min="8" max="8" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.8125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.3984375" customWidth="1"/>
+    <col min="3" max="3" width="34.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.19921875" customWidth="1"/>
+    <col min="8" max="8" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.7">
-      <c r="A3" t="s">
-        <v>42</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1031,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D4">
         <v>1</v>
       </c>
@@ -1042,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D5">
         <v>4</v>
       </c>
@@ -1050,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E6">
         <v>6</v>
       </c>

</xml_diff>